<commit_message>
Final Commit from home 9/17
</commit_message>
<xml_diff>
--- a/Application 2/PandasCSV/supermarkets.xlsx
+++ b/Application 2/PandasCSV/supermarkets.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F949BF4-45BF-4B2E-A50F-797D2EA0D53C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -33,9 +34,6 @@
     <t>Country</t>
   </si>
   <si>
-    <t>Supermarket Name</t>
-  </si>
-  <si>
     <t>Number of Employees</t>
   </si>
   <si>
@@ -91,12 +89,15 @@
   </si>
   <si>
     <t>Ben's Shop</t>
+  </si>
+  <si>
+    <t>Name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -137,6 +138,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -185,7 +189,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -218,9 +222,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -253,6 +274,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -428,11 +466,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -454,10 +492,10 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -465,19 +503,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G2">
         <v>8</v>
@@ -488,19 +526,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G3">
         <v>15</v>
@@ -511,19 +549,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
         <v>7</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>8</v>
       </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
       <c r="F4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G4">
         <v>25</v>
@@ -534,19 +572,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G5">
         <v>10</v>
@@ -557,19 +595,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
         <v>10</v>
       </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" t="s">
         <v>11</v>
-      </c>
-      <c r="E6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" t="s">
-        <v>12</v>
       </c>
       <c r="G6">
         <v>12</v>
@@ -580,19 +618,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
         <v>13</v>
       </c>
-      <c r="C7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" t="s">
         <v>14</v>
-      </c>
-      <c r="E7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" t="s">
-        <v>15</v>
       </c>
       <c r="G7">
         <v>20</v>
@@ -604,7 +642,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -616,7 +654,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>